<commit_message>
Lab 2 edits (Liz suggestions)
</commit_message>
<xml_diff>
--- a/assignments/Lab2_Tables.xlsx
+++ b/assignments/Lab2_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18165\Documents\R\Lab\biostatlab\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D3B236-9498-4ABE-93B4-391B497C48C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34004177-B2FD-49BE-9D55-0339A9289296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1170" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0FAFAFAC-844D-4B83-80DB-945B6FD3464C}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0FAFAFAC-844D-4B83-80DB-945B6FD3464C}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1, Frequency distribution" sheetId="1" r:id="rId1"/>
@@ -922,7 +922,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1007,8 +1010,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1021,8 +1046,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8D0D0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1048,15 +1115,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1160,52 +1218,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1213,194 +1357,427 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
+    <cellStyle name="20% - Accent6" xfId="5" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF8D0D0"/>
+      <color rgb="FFF19999"/>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FF767171"/>
     </mruColors>
   </colors>
@@ -1413,6 +1790,170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>125730</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Brace 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8416D2F2-83F1-4772-8A64-F29116486B2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9336405" y="16097250"/>
+          <a:ext cx="331470" cy="2087880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>49530</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6610F8D-D363-4F1A-8C7C-A32A6C60BEB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9869805" y="16474440"/>
+          <a:ext cx="3760470" cy="1487805"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="28575" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="8100000" algn="tr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2500" b="1" u="sng"/>
+            <a:t>Copy</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2500"/>
+            <a:t> the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2500" baseline="0"/>
+            <a:t> 7 new rows you created in Table 2 for Lab 1 and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2500" b="1" u="sng" baseline="0"/>
+            <a:t>paste</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2500" baseline="0"/>
+            <a:t> them here. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2500"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1715,7 +2256,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1727,227 +2268,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="90"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="54"/>
+      <c r="D7" s="54" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="35"/>
+      <c r="B9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="63"/>
+      <c r="B10" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="65"/>
+      <c r="D10" s="65" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="69"/>
+      <c r="B13" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="71" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="37"/>
+      <c r="B15" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="75"/>
+      <c r="B16" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="77"/>
+      <c r="D16" s="77" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="81"/>
+      <c r="B20" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="83"/>
+      <c r="D20" s="83" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="87"/>
+      <c r="B23" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6" t="s">
+      <c r="C23" s="89"/>
+      <c r="D23" s="89" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1959,853 +2500,853 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46:F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="16" customWidth="1"/>
-    <col min="5" max="6" width="12.88671875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11" style="16" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="19.21875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="7" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
     </row>
     <row r="4" spans="1:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="12" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
     </row>
     <row r="7" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="12" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="95"/>
+      <c r="I8" s="95"/>
     </row>
     <row r="9" spans="1:9" ht="132.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="14" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="93"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="11" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="11" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="11" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="102"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="11" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="11" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="102"/>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="12" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="95"/>
     </row>
     <row r="19" spans="1:9" ht="132.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="92"/>
     </row>
     <row r="20" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92"/>
     </row>
     <row r="21" spans="1:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92"/>
     </row>
     <row r="22" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="93"/>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="12" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="95"/>
     </row>
     <row r="24" spans="1:9" ht="145.80000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
     </row>
     <row r="25" spans="1:9" ht="145.80000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="97"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="13" t="s">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="49"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="14" t="s">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="99"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="57"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="93"/>
+      <c r="I29" s="93"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="11" t="s">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
+      <c r="D30" s="102"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="102"/>
+      <c r="I30" s="102"/>
     </row>
     <row r="31" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="11" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="102"/>
+      <c r="I31" s="102"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="11" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="66"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
+      <c r="D32" s="102"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="102"/>
+      <c r="I32" s="102"/>
     </row>
     <row r="33" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="51"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="11" t="s">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="66"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
+      <c r="D33" s="102"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="49"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="12" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="95"/>
+      <c r="I34" s="95"/>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="46"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
+      <c r="A35" s="123"/>
+      <c r="B35" s="124"/>
+      <c r="C35" s="124"/>
+      <c r="D35" s="125"/>
+      <c r="E35" s="125"/>
+      <c r="F35" s="125"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="125"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="47"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
+      <c r="A36" s="126"/>
+      <c r="B36" s="127"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="129"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="51"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
+      <c r="A37" s="130"/>
+      <c r="B37" s="131"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="132"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="132"/>
+      <c r="G37" s="132"/>
+      <c r="H37" s="132"/>
+      <c r="I37" s="132"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="59"/>
+      <c r="A38" s="133"/>
+      <c r="B38" s="134"/>
+      <c r="C38" s="135"/>
+      <c r="D38" s="136"/>
+      <c r="E38" s="136"/>
+      <c r="F38" s="136"/>
+      <c r="G38" s="136"/>
+      <c r="H38" s="136"/>
+      <c r="I38" s="136"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
+      <c r="A39" s="123"/>
+      <c r="B39" s="124"/>
+      <c r="C39" s="124"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="125"/>
+      <c r="F39" s="125"/>
+      <c r="G39" s="125"/>
+      <c r="H39" s="125"/>
+      <c r="I39" s="125"/>
     </row>
     <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="46"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
+      <c r="A40" s="123"/>
+      <c r="B40" s="124"/>
+      <c r="C40" s="124"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="125"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="125"/>
+      <c r="I40" s="125"/>
     </row>
     <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="46"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
+      <c r="A41" s="123"/>
+      <c r="B41" s="124"/>
+      <c r="C41" s="124"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="125"/>
+      <c r="F41" s="125"/>
+      <c r="G41" s="125"/>
+      <c r="H41" s="125"/>
+      <c r="I41" s="125"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="47"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="57"/>
-      <c r="I42" s="57"/>
+      <c r="A42" s="126"/>
+      <c r="B42" s="127"/>
+      <c r="C42" s="128"/>
+      <c r="D42" s="129"/>
+      <c r="E42" s="129"/>
+      <c r="F42" s="129"/>
+      <c r="G42" s="129"/>
+      <c r="H42" s="129"/>
+      <c r="I42" s="129"/>
     </row>
     <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="49"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
+      <c r="A43" s="133"/>
+      <c r="B43" s="134"/>
+      <c r="C43" s="135"/>
+      <c r="D43" s="136"/>
+      <c r="E43" s="136"/>
+      <c r="F43" s="136"/>
+      <c r="G43" s="136"/>
+      <c r="H43" s="136"/>
+      <c r="I43" s="136"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
+      <c r="A44" s="137"/>
+      <c r="B44" s="137"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="139"/>
+      <c r="E44" s="140"/>
+      <c r="F44" s="139"/>
+      <c r="G44" s="139"/>
+      <c r="H44" s="139"/>
+      <c r="I44" s="139"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
+      <c r="A45" s="141"/>
+      <c r="B45" s="141"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="142"/>
+      <c r="E45" s="143"/>
+      <c r="F45" s="142"/>
+      <c r="G45" s="142"/>
+      <c r="H45" s="142"/>
+      <c r="I45" s="142"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="33"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="109"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
+      <c r="H46" s="108"/>
+      <c r="I46" s="108"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="35"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="113"/>
+      <c r="F47" s="113"/>
+      <c r="G47" s="113"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="112"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="35"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="112"/>
+      <c r="E48" s="113"/>
+      <c r="F48" s="113"/>
+      <c r="G48" s="113"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="112"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="35"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="112"/>
+      <c r="E49" s="113"/>
+      <c r="F49" s="113"/>
+      <c r="G49" s="113"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="112"/>
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="37"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="110"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="110"/>
+      <c r="I50" s="110"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="33"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="108"/>
+      <c r="E51" s="109"/>
+      <c r="F51" s="109"/>
+      <c r="G51" s="109"/>
+      <c r="H51" s="108"/>
+      <c r="I51" s="108"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="37"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="110"/>
+      <c r="E52" s="111"/>
+      <c r="F52" s="111"/>
+      <c r="G52" s="111"/>
+      <c r="H52" s="110"/>
+      <c r="I52" s="110"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="33"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="108"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="108"/>
+      <c r="I53" s="108"/>
     </row>
     <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="110"/>
+      <c r="E54" s="111"/>
+      <c r="F54" s="111"/>
+      <c r="G54" s="111"/>
+      <c r="H54" s="110"/>
+      <c r="I54" s="110"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="33"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="108"/>
+      <c r="E55" s="109"/>
+      <c r="F55" s="109"/>
+      <c r="G55" s="109"/>
+      <c r="H55" s="108"/>
+      <c r="I55" s="108"/>
     </row>
     <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="37"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="110"/>
+      <c r="E56" s="111"/>
+      <c r="F56" s="111"/>
+      <c r="G56" s="111"/>
+      <c r="H56" s="110"/>
+      <c r="I56" s="110"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="33"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="108"/>
+      <c r="E57" s="109"/>
+      <c r="F57" s="109"/>
+      <c r="G57" s="109"/>
+      <c r="H57" s="108"/>
+      <c r="I57" s="108"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="35"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="112"/>
+      <c r="E58" s="113"/>
+      <c r="F58" s="113"/>
+      <c r="G58" s="113"/>
+      <c r="H58" s="112"/>
+      <c r="I58" s="112"/>
     </row>
     <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="37"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="110"/>
+      <c r="E59" s="111"/>
+      <c r="F59" s="111"/>
+      <c r="G59" s="111"/>
+      <c r="H59" s="110"/>
+      <c r="I59" s="110"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="39"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="29"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="114"/>
+      <c r="E60" s="115"/>
+      <c r="F60" s="115"/>
+      <c r="G60" s="115"/>
+      <c r="H60" s="114"/>
+      <c r="I60" s="114"/>
     </row>
     <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="42"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="31"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="116"/>
+      <c r="E61" s="117"/>
+      <c r="F61" s="117"/>
+      <c r="G61" s="117"/>
+      <c r="H61" s="116"/>
+      <c r="I61" s="116"/>
     </row>
     <row r="62" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="53"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="75"/>
-      <c r="G62" s="76"/>
-      <c r="H62" s="73"/>
-      <c r="I62" s="77"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="118"/>
+      <c r="E62" s="119"/>
+      <c r="F62" s="120"/>
+      <c r="G62" s="121"/>
+      <c r="H62" s="118"/>
+      <c r="I62" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="128">
@@ -2820,6 +3361,9 @@
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="G60:G61"/>
     <mergeCell ref="H60:H61"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="E51:E52"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="F53:F54"/>
     <mergeCell ref="G53:G54"/>
@@ -2830,17 +3374,6 @@
     <mergeCell ref="D57:D59"/>
     <mergeCell ref="E57:E59"/>
     <mergeCell ref="F57:F59"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="E51:E52"/>
     <mergeCell ref="H46:H50"/>
     <mergeCell ref="I46:I50"/>
     <mergeCell ref="A55:A56"/>
@@ -2857,6 +3390,14 @@
     <mergeCell ref="E46:E50"/>
     <mergeCell ref="F46:F50"/>
     <mergeCell ref="G46:G50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="I51:I52"/>
     <mergeCell ref="H42:H43"/>
     <mergeCell ref="I42:I43"/>
     <mergeCell ref="A44:A45"/>
@@ -2940,5 +3481,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>